<commit_message>
Added a script for numpy's average execution time calculation which generate an xlsx file with tables
</commit_message>
<xml_diff>
--- a/execution_results/add_sub_exec_times_table.xlsx
+++ b/execution_results/add_sub_exec_times_table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="23">
   <si>
     <t>Addition and Subtraction time</t>
   </si>
@@ -52,16 +52,31 @@
     <t>10000</t>
   </si>
   <si>
+    <t>11000</t>
+  </si>
+  <si>
+    <t>12000</t>
+  </si>
+  <si>
+    <t>13000</t>
+  </si>
+  <si>
+    <t>14000</t>
+  </si>
+  <si>
+    <t>15000</t>
+  </si>
+  <si>
     <t>addition_csr</t>
   </si>
   <si>
-    <t>subtration_csr</t>
+    <t>subtraction_csr</t>
   </si>
   <si>
     <t>addition_csc</t>
   </si>
   <si>
-    <t>subtration_csc</t>
+    <t>subtraction_csc</t>
   </si>
   <si>
     <t>0.01</t>
@@ -118,9 +133,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:L7" totalsRowShown="0">
-  <autoFilter ref="B3:L7"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:Q7" totalsRowShown="0">
+  <autoFilter ref="B3:Q7"/>
+  <tableColumns count="16">
     <tableColumn id="1" name="0.005"/>
     <tableColumn id="2" name="1000" dataDxfId="0"/>
     <tableColumn id="3" name="2000" dataDxfId="0"/>
@@ -132,15 +147,20 @@
     <tableColumn id="9" name="8000" dataDxfId="0"/>
     <tableColumn id="10" name="9000" dataDxfId="0"/>
     <tableColumn id="11" name="10000" dataDxfId="0"/>
+    <tableColumn id="12" name="11000" dataDxfId="0"/>
+    <tableColumn id="13" name="12000" dataDxfId="0"/>
+    <tableColumn id="14" name="13000" dataDxfId="0"/>
+    <tableColumn id="15" name="14000" dataDxfId="0"/>
+    <tableColumn id="16" name="15000" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B11:L15" totalsRowShown="0">
-  <autoFilter ref="B11:L15"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B11:Q15" totalsRowShown="0">
+  <autoFilter ref="B11:Q15"/>
+  <tableColumns count="16">
     <tableColumn id="1" name="0.01"/>
     <tableColumn id="2" name="1000" dataDxfId="0"/>
     <tableColumn id="3" name="2000" dataDxfId="0"/>
@@ -152,15 +172,20 @@
     <tableColumn id="9" name="8000" dataDxfId="0"/>
     <tableColumn id="10" name="9000" dataDxfId="0"/>
     <tableColumn id="11" name="10000" dataDxfId="0"/>
+    <tableColumn id="12" name="11000" dataDxfId="0"/>
+    <tableColumn id="13" name="12000" dataDxfId="0"/>
+    <tableColumn id="14" name="13000" dataDxfId="0"/>
+    <tableColumn id="15" name="14000" dataDxfId="0"/>
+    <tableColumn id="16" name="15000" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B19:L23" totalsRowShown="0">
-  <autoFilter ref="B19:L23"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B19:Q23" totalsRowShown="0">
+  <autoFilter ref="B19:Q23"/>
+  <tableColumns count="16">
     <tableColumn id="1" name="0.02"/>
     <tableColumn id="2" name="1000" dataDxfId="0"/>
     <tableColumn id="3" name="2000" dataDxfId="0"/>
@@ -172,6 +197,11 @@
     <tableColumn id="9" name="8000" dataDxfId="0"/>
     <tableColumn id="10" name="9000" dataDxfId="0"/>
     <tableColumn id="11" name="10000" dataDxfId="0"/>
+    <tableColumn id="12" name="11000" dataDxfId="0"/>
+    <tableColumn id="13" name="12000" dataDxfId="0"/>
+    <tableColumn id="14" name="13000" dataDxfId="0"/>
+    <tableColumn id="15" name="14000" dataDxfId="0"/>
+    <tableColumn id="16" name="15000" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -462,7 +492,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:L23"/>
+  <dimension ref="B1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -471,12 +501,12 @@
     <col min="2" max="6" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12">
+    <row r="1" spans="2:17">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:12">
+    <row r="3" spans="2:17">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -510,150 +540,225 @@
       <c r="L3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="2:12">
+      <c r="M3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17">
       <c r="B4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1">
-        <v>0.00769</v>
+        <v>0.007923999999999999</v>
       </c>
       <c r="D4" s="1">
-        <v>0.026817</v>
+        <v>0.027088</v>
       </c>
       <c r="E4" s="1">
-        <v>0.06005400000000001</v>
+        <v>0.06057100000000001</v>
       </c>
       <c r="F4" s="1">
-        <v>0.11169</v>
+        <v>0.113555</v>
       </c>
       <c r="G4" s="1">
-        <v>0.181758</v>
+        <v>0.181902</v>
       </c>
       <c r="H4" s="1">
-        <v>0.2727939999999999</v>
+        <v>0.274877</v>
       </c>
       <c r="I4" s="1">
-        <v>0.388677</v>
+        <v>0.3962290000000001</v>
       </c>
       <c r="J4" s="1">
-        <v>0.534962</v>
+        <v>0.539411</v>
       </c>
       <c r="K4" s="1">
-        <v>0.7069360000000001</v>
+        <v>0.7195550000000001</v>
       </c>
       <c r="L4" s="1">
-        <v>0.8159040000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12">
+        <v>0.9307650000000001</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1.198896</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1.445078</v>
+      </c>
+      <c r="O4" s="1">
+        <v>1.769522</v>
+      </c>
+      <c r="P4" s="1">
+        <v>2.139689</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>2.554645</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17">
       <c r="B5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1">
-        <v>0.00808</v>
+        <v>0.008118</v>
       </c>
       <c r="D5" s="1">
-        <v>0.027606</v>
+        <v>0.027634</v>
       </c>
       <c r="E5" s="1">
-        <v>0.06148199999999999</v>
+        <v>0.06273199999999998</v>
       </c>
       <c r="F5" s="1">
-        <v>0.115808</v>
+        <v>0.119001</v>
       </c>
       <c r="G5" s="1">
-        <v>0.19023</v>
+        <v>0.191547</v>
       </c>
       <c r="H5" s="1">
-        <v>0.282263</v>
+        <v>0.287118</v>
       </c>
       <c r="I5" s="1">
-        <v>0.3965029999999999</v>
+        <v>0.407289</v>
       </c>
       <c r="J5" s="1">
-        <v>0.5438949999999999</v>
+        <v>0.551316</v>
       </c>
       <c r="K5" s="1">
-        <v>0.718007</v>
+        <v>0.737119</v>
       </c>
       <c r="L5" s="1">
-        <v>0.8223670000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12">
+        <v>0.953928</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1.197954</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1.460427</v>
+      </c>
+      <c r="O5" s="1">
+        <v>1.778972</v>
+      </c>
+      <c r="P5" s="1">
+        <v>2.166445</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>2.594647</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17">
       <c r="B6" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1">
-        <v>0.007828999999999999</v>
+        <v>0.008089000000000001</v>
       </c>
       <c r="D6" s="1">
-        <v>0.02829600000000001</v>
+        <v>0.027413</v>
       </c>
       <c r="E6" s="1">
-        <v>0.061463</v>
+        <v>0.063056</v>
       </c>
       <c r="F6" s="1">
-        <v>0.116585</v>
+        <v>0.118821</v>
       </c>
       <c r="G6" s="1">
-        <v>0.188884</v>
+        <v>0.191288</v>
       </c>
       <c r="H6" s="1">
-        <v>0.280976</v>
+        <v>0.284725</v>
       </c>
       <c r="I6" s="1">
-        <v>0.396442</v>
+        <v>0.409952</v>
       </c>
       <c r="J6" s="1">
-        <v>0.543205</v>
+        <v>0.5561160000000001</v>
       </c>
       <c r="K6" s="1">
-        <v>0.7167000000000001</v>
+        <v>0.7298980000000002</v>
       </c>
       <c r="L6" s="1">
-        <v>0.821669</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12">
+        <v>0.9400960000000002</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1.180584</v>
+      </c>
+      <c r="N6" s="1">
+        <v>1.456368</v>
+      </c>
+      <c r="O6" s="1">
+        <v>1.779277</v>
+      </c>
+      <c r="P6" s="1">
+        <v>2.152697</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>2.599839</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17">
       <c r="B7" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1">
-        <v>0.007872000000000001</v>
+        <v>0.008193000000000001</v>
       </c>
       <c r="D7" s="1">
-        <v>0.027625</v>
+        <v>0.028129</v>
       </c>
       <c r="E7" s="1">
-        <v>0.062419</v>
+        <v>0.063433</v>
       </c>
       <c r="F7" s="1">
-        <v>0.118154</v>
+        <v>0.118838</v>
       </c>
       <c r="G7" s="1">
-        <v>0.192357</v>
+        <v>0.195204</v>
       </c>
       <c r="H7" s="1">
-        <v>0.285159</v>
+        <v>0.291445</v>
       </c>
       <c r="I7" s="1">
-        <v>0.404313</v>
+        <v>0.4118709999999999</v>
       </c>
       <c r="J7" s="1">
-        <v>0.5540849999999999</v>
+        <v>0.560257</v>
       </c>
       <c r="K7" s="1">
-        <v>0.7301749999999999</v>
+        <v>0.746381</v>
       </c>
       <c r="L7" s="1">
-        <v>0.8376809999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12">
+        <v>0.953993</v>
+      </c>
+      <c r="M7" s="1">
+        <v>1.20354</v>
+      </c>
+      <c r="N7" s="1">
+        <v>1.474232</v>
+      </c>
+      <c r="O7" s="1">
+        <v>1.822403</v>
+      </c>
+      <c r="P7" s="1">
+        <v>2.207352</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>2.658625</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17">
       <c r="B11" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -685,150 +790,225 @@
       <c r="L11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="2:12">
+      <c r="M11" t="s">
+        <v>12</v>
+      </c>
+      <c r="N11" t="s">
+        <v>13</v>
+      </c>
+      <c r="O11" t="s">
+        <v>14</v>
+      </c>
+      <c r="P11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17">
       <c r="B12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C12" s="1">
-        <v>0.0136</v>
+        <v>0.014075</v>
       </c>
       <c r="D12" s="1">
-        <v>0.05522900000000001</v>
+        <v>0.05599</v>
       </c>
       <c r="E12" s="1">
-        <v>0.135275</v>
+        <v>0.138048</v>
       </c>
       <c r="F12" s="1">
-        <v>0.266115</v>
+        <v>0.271246</v>
       </c>
       <c r="G12" s="1">
-        <v>0.4544029999999999</v>
+        <v>0.464772</v>
       </c>
       <c r="H12" s="1">
-        <v>0.71187</v>
+        <v>0.730065</v>
       </c>
       <c r="I12" s="1">
-        <v>1.057717</v>
+        <v>1.081819</v>
       </c>
       <c r="J12" s="1">
-        <v>1.49495</v>
+        <v>1.522875</v>
       </c>
       <c r="K12" s="1">
-        <v>2.035084</v>
+        <v>2.07307</v>
       </c>
       <c r="L12" s="1">
-        <v>2.387926</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12">
+        <v>2.735982</v>
+      </c>
+      <c r="M12" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="N12" s="1">
+        <v>4.342772</v>
+      </c>
+      <c r="O12" s="1">
+        <v>5.358774</v>
+      </c>
+      <c r="P12" s="1">
+        <v>6.547840000000001</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>7.883540999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17">
       <c r="B13" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C13" s="1">
-        <v>0.014104</v>
+        <v>0.014366</v>
       </c>
       <c r="D13" s="1">
-        <v>0.057946</v>
+        <v>0.058123</v>
       </c>
       <c r="E13" s="1">
-        <v>0.139616</v>
+        <v>0.142464</v>
       </c>
       <c r="F13" s="1">
-        <v>0.270764</v>
+        <v>0.276263</v>
       </c>
       <c r="G13" s="1">
-        <v>0.466071</v>
+        <v>0.476504</v>
       </c>
       <c r="H13" s="1">
-        <v>0.718708</v>
+        <v>0.738939</v>
       </c>
       <c r="I13" s="1">
-        <v>1.069224</v>
+        <v>1.088414</v>
       </c>
       <c r="J13" s="1">
-        <v>1.539019</v>
+        <v>1.565037</v>
       </c>
       <c r="K13" s="1">
-        <v>2.081244</v>
+        <v>2.140165</v>
       </c>
       <c r="L13" s="1">
-        <v>2.447348</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12">
+        <v>2.801308</v>
+      </c>
+      <c r="M13" s="1">
+        <v>3.570284</v>
+      </c>
+      <c r="N13" s="1">
+        <v>4.426456</v>
+      </c>
+      <c r="O13" s="1">
+        <v>5.433976</v>
+      </c>
+      <c r="P13" s="1">
+        <v>6.631990999999999</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>7.992939</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17">
       <c r="B14" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C14" s="1">
-        <v>0.013836</v>
+        <v>0.013909</v>
       </c>
       <c r="D14" s="1">
-        <v>0.058348</v>
+        <v>0.058607</v>
       </c>
       <c r="E14" s="1">
-        <v>0.139379</v>
+        <v>0.141561</v>
       </c>
       <c r="F14" s="1">
-        <v>0.270031</v>
+        <v>0.276364</v>
       </c>
       <c r="G14" s="1">
-        <v>0.461323</v>
+        <v>0.4712370000000001</v>
       </c>
       <c r="H14" s="1">
-        <v>0.7168880000000001</v>
+        <v>0.7344269999999999</v>
       </c>
       <c r="I14" s="1">
-        <v>1.071891</v>
+        <v>1.096746</v>
       </c>
       <c r="J14" s="1">
-        <v>1.525824</v>
+        <v>1.569738</v>
       </c>
       <c r="K14" s="1">
-        <v>2.075977</v>
+        <v>2.121854</v>
       </c>
       <c r="L14" s="1">
-        <v>2.437472</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12">
+        <v>2.783945</v>
+      </c>
+      <c r="M14" s="1">
+        <v>3.555473999999999</v>
+      </c>
+      <c r="N14" s="1">
+        <v>4.394168000000001</v>
+      </c>
+      <c r="O14" s="1">
+        <v>5.433046</v>
+      </c>
+      <c r="P14" s="1">
+        <v>6.586393000000001</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>7.957806</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17">
       <c r="B15" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C15" s="1">
-        <v>0.013927</v>
+        <v>0.014066</v>
       </c>
       <c r="D15" s="1">
-        <v>0.058341</v>
+        <v>0.05985500000000001</v>
       </c>
       <c r="E15" s="1">
-        <v>0.14177</v>
+        <v>0.145239</v>
       </c>
       <c r="F15" s="1">
-        <v>0.274818</v>
+        <v>0.281807</v>
       </c>
       <c r="G15" s="1">
-        <v>0.4696239999999999</v>
+        <v>0.476622</v>
       </c>
       <c r="H15" s="1">
-        <v>0.730196</v>
+        <v>0.7428239999999999</v>
       </c>
       <c r="I15" s="1">
-        <v>1.090288</v>
+        <v>1.126362</v>
       </c>
       <c r="J15" s="1">
-        <v>1.55677</v>
+        <v>1.601466</v>
       </c>
       <c r="K15" s="1">
-        <v>2.116079</v>
+        <v>2.170681</v>
       </c>
       <c r="L15" s="1">
-        <v>2.487459</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12">
+        <v>2.846819</v>
+      </c>
+      <c r="M15" s="1">
+        <v>3.631046</v>
+      </c>
+      <c r="N15" s="1">
+        <v>4.494356000000001</v>
+      </c>
+      <c r="O15" s="1">
+        <v>5.54616</v>
+      </c>
+      <c r="P15" s="1">
+        <v>6.726816000000001</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>8.10455</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17">
       <c r="B19" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
@@ -860,145 +1040,220 @@
       <c r="L19" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="2:12">
+      <c r="M19" t="s">
+        <v>12</v>
+      </c>
+      <c r="N19" t="s">
+        <v>13</v>
+      </c>
+      <c r="O19" t="s">
+        <v>14</v>
+      </c>
+      <c r="P19" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17">
       <c r="B20" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C20" s="1">
-        <v>0.029069</v>
+        <v>0.029756</v>
       </c>
       <c r="D20" s="1">
-        <v>0.133191</v>
+        <v>0.133935</v>
       </c>
       <c r="E20" s="1">
-        <v>0.354311</v>
+        <v>0.361437</v>
       </c>
       <c r="F20" s="1">
-        <v>0.742882</v>
+        <v>0.7646379999999999</v>
       </c>
       <c r="G20" s="1">
-        <v>1.325181</v>
+        <v>1.357092</v>
       </c>
       <c r="H20" s="1">
-        <v>2.13281</v>
+        <v>2.187737</v>
       </c>
       <c r="I20" s="1">
-        <v>3.224823</v>
+        <v>3.293286</v>
       </c>
       <c r="J20" s="1">
-        <v>4.630822999999999</v>
+        <v>4.740823000000001</v>
       </c>
       <c r="K20" s="1">
-        <v>6.390786</v>
+        <v>6.539346</v>
       </c>
       <c r="L20" s="1">
-        <v>7.643555000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12">
+        <v>8.743188999999997</v>
+      </c>
+      <c r="M20" s="1">
+        <v>11.358781</v>
+      </c>
+      <c r="N20" s="1">
+        <v>14.370211</v>
+      </c>
+      <c r="O20" s="1">
+        <v>17.920053</v>
+      </c>
+      <c r="P20" s="1">
+        <v>22.218637</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>29.049141</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17">
       <c r="B21" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C21" s="1">
-        <v>0.030574</v>
+        <v>0.03153499999999999</v>
       </c>
       <c r="D21" s="1">
-        <v>0.135359</v>
+        <v>0.136268</v>
       </c>
       <c r="E21" s="1">
-        <v>0.3613430000000001</v>
+        <v>0.363836</v>
       </c>
       <c r="F21" s="1">
-        <v>0.7578889999999999</v>
+        <v>0.772818</v>
       </c>
       <c r="G21" s="1">
-        <v>1.360648</v>
+        <v>1.387557</v>
       </c>
       <c r="H21" s="1">
-        <v>2.169031</v>
+        <v>2.231125</v>
       </c>
       <c r="I21" s="1">
-        <v>3.257579</v>
+        <v>3.309132</v>
       </c>
       <c r="J21" s="1">
-        <v>4.822445999999999</v>
+        <v>4.802413</v>
       </c>
       <c r="K21" s="1">
-        <v>6.446786999999999</v>
+        <v>6.590045000000001</v>
       </c>
       <c r="L21" s="1">
-        <v>7.688557999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12">
+        <v>8.767270999999999</v>
+      </c>
+      <c r="M21" s="1">
+        <v>11.412014</v>
+      </c>
+      <c r="N21" s="1">
+        <v>14.415702</v>
+      </c>
+      <c r="O21" s="1">
+        <v>18.048974</v>
+      </c>
+      <c r="P21" s="1">
+        <v>22.302494</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>29.116331</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17">
       <c r="B22" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C22" s="1">
-        <v>0.029487</v>
+        <v>0.029429</v>
       </c>
       <c r="D22" s="1">
-        <v>0.134174</v>
+        <v>0.13759</v>
       </c>
       <c r="E22" s="1">
-        <v>0.36102</v>
+        <v>0.364102</v>
       </c>
       <c r="F22" s="1">
-        <v>0.7574899999999999</v>
+        <v>0.777284</v>
       </c>
       <c r="G22" s="1">
-        <v>1.35137</v>
+        <v>1.386954</v>
       </c>
       <c r="H22" s="1">
-        <v>2.171955</v>
+        <v>2.220994999999999</v>
       </c>
       <c r="I22" s="1">
-        <v>3.241131999999999</v>
+        <v>3.323858</v>
       </c>
       <c r="J22" s="1">
-        <v>4.671797</v>
+        <v>4.760835</v>
       </c>
       <c r="K22" s="1">
-        <v>6.447685</v>
+        <v>6.57149</v>
       </c>
       <c r="L22" s="1">
-        <v>7.711152999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12">
+        <v>8.805575999999999</v>
+      </c>
+      <c r="M22" s="1">
+        <v>11.438485</v>
+      </c>
+      <c r="N22" s="1">
+        <v>14.377479</v>
+      </c>
+      <c r="O22" s="1">
+        <v>17.987201</v>
+      </c>
+      <c r="P22" s="1">
+        <v>22.155565</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>28.877955</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17">
       <c r="B23" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C23" s="1">
-        <v>0.029041</v>
+        <v>0.02991899999999999</v>
       </c>
       <c r="D23" s="1">
-        <v>0.136752</v>
+        <v>0.139802</v>
       </c>
       <c r="E23" s="1">
-        <v>0.367725</v>
+        <v>0.3741420000000001</v>
       </c>
       <c r="F23" s="1">
-        <v>0.776218</v>
+        <v>0.785755</v>
       </c>
       <c r="G23" s="1">
-        <v>1.388719</v>
+        <v>1.416995</v>
       </c>
       <c r="H23" s="1">
-        <v>2.212999</v>
+        <v>2.269072</v>
       </c>
       <c r="I23" s="1">
-        <v>3.30458</v>
+        <v>3.375549</v>
       </c>
       <c r="J23" s="1">
-        <v>4.773662</v>
+        <v>4.830209999999999</v>
       </c>
       <c r="K23" s="1">
-        <v>6.54753</v>
+        <v>6.690988</v>
       </c>
       <c r="L23" s="1">
-        <v>7.817624</v>
+        <v>8.916752999999998</v>
+      </c>
+      <c r="M23" s="1">
+        <v>11.57588</v>
+      </c>
+      <c r="N23" s="1">
+        <v>14.547477</v>
+      </c>
+      <c r="O23" s="1">
+        <v>18.204949</v>
+      </c>
+      <c r="P23" s="1">
+        <v>22.404405</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>29.416086</v>
       </c>
     </row>
   </sheetData>

</xml_diff>